<commit_message>
Compleate Plot diagram script
</commit_message>
<xml_diff>
--- a/bin/Ph-N2+-MTMO-transform.xlsx
+++ b/bin/Ph-N2+-MTMO-transform.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="18">
   <si>
     <t xml:space="preserve">MinE_MO</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve"> E_Frag_MO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Occup</t>
   </si>
   <si>
     <t xml:space="preserve">Frag</t>
@@ -299,10 +302,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I45" activeCellId="0" sqref="I45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -313,11 +316,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="38.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="38.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,8 +352,11 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -371,18 +378,21 @@
       <c r="F2" s="5" t="n">
         <v>-14.441894</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>10</v>
+      <c r="G2" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="n">
         <f aca="false">B2-F2</f>
         <v>-0.289026</v>
       </c>
-      <c r="J2" s="7" t="n">
-        <f aca="false">I2*100/1.318538</f>
+      <c r="K2" s="7" t="n">
+        <f aca="false">J2*100/1.318538</f>
         <v>-21.9201873590295</v>
       </c>
     </row>
@@ -405,18 +415,21 @@
       <c r="F3" s="5" t="n">
         <v>-14.440486</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
+      <c r="G3" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="5" t="n">
         <f aca="false">B3-F3</f>
         <v>-0.255304000000001</v>
       </c>
-      <c r="J3" s="7" t="n">
-        <f aca="false">I3*100/1.318538</f>
+      <c r="K3" s="7" t="n">
+        <f aca="false">J3*100/1.318538</f>
         <v>-19.3626577315178</v>
       </c>
     </row>
@@ -439,18 +452,21 @@
       <c r="F4" s="8" t="n">
         <v>-10.521741</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>12</v>
+      <c r="G4" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="8" t="n">
+      <c r="I4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="8" t="n">
         <f aca="false">B4-F4</f>
         <v>0.0465809999999998</v>
       </c>
-      <c r="J4" s="10" t="n">
-        <f aca="false">I4*100/1.318538</f>
+      <c r="K4" s="10" t="n">
+        <f aca="false">J4*100/1.318538</f>
         <v>3.53277645392092</v>
       </c>
     </row>
@@ -473,18 +489,21 @@
       <c r="F5" s="8" t="n">
         <v>-10.446997</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>12</v>
+      <c r="G5" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="8" t="n">
+      <c r="I5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="8" t="n">
         <f aca="false">B5-F5</f>
         <v>0.0340969999999992</v>
       </c>
-      <c r="J5" s="10" t="n">
-        <f aca="false">I5*100/1.318538</f>
+      <c r="K5" s="10" t="n">
+        <f aca="false">J5*100/1.318538</f>
         <v>2.58597021852985</v>
       </c>
     </row>
@@ -507,18 +526,21 @@
       <c r="F6" s="8" t="n">
         <v>-10.446928</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>12</v>
+      <c r="G6" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="I6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="8" t="n">
         <f aca="false">B6-F6</f>
         <v>0.0341079999999998</v>
       </c>
-      <c r="J6" s="10" t="n">
-        <f aca="false">I6*100/1.318538</f>
+      <c r="K6" s="10" t="n">
+        <f aca="false">J6*100/1.318538</f>
         <v>2.58680447586644</v>
       </c>
     </row>
@@ -541,18 +563,21 @@
       <c r="F7" s="8" t="n">
         <v>-10.433769</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>12</v>
+      <c r="G7" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="8" t="n">
+      <c r="I7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="8" t="n">
         <f aca="false">B7-F7</f>
         <v>0.0391589999999997</v>
       </c>
-      <c r="J7" s="10" t="n">
-        <f aca="false">I7*100/1.318538</f>
+      <c r="K7" s="10" t="n">
+        <f aca="false">J7*100/1.318538</f>
         <v>2.96988027648803</v>
       </c>
     </row>
@@ -575,18 +600,21 @@
       <c r="F8" s="8" t="n">
         <v>-10.433741</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>12</v>
+      <c r="G8" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="8" t="n">
+      <c r="I8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="8" t="n">
         <f aca="false">B8-F8</f>
         <v>0.0467709999999997</v>
       </c>
-      <c r="J8" s="10" t="n">
-        <f aca="false">I8*100/1.318538</f>
+      <c r="K8" s="10" t="n">
+        <f aca="false">J8*100/1.318538</f>
         <v>3.54718635337015</v>
       </c>
     </row>
@@ -609,18 +637,21 @@
       <c r="F9" s="8" t="n">
         <v>-10.406684</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>12</v>
+      <c r="G9" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="I9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="8" t="n">
         <f aca="false">B9-F9</f>
         <v>0.0197540000000007</v>
       </c>
-      <c r="J9" s="10" t="n">
-        <f aca="false">I9*100/1.318538</f>
+      <c r="K9" s="10" t="n">
+        <f aca="false">J9*100/1.318538</f>
         <v>1.49817449326456</v>
       </c>
     </row>
@@ -643,18 +674,21 @@
       <c r="F10" s="5" t="n">
         <v>-1.123113</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>10</v>
+      <c r="G10" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="5" t="n">
         <f aca="false">B10-F10</f>
         <v>-0.258127</v>
       </c>
-      <c r="J10" s="7" t="n">
-        <f aca="false">I10*100/1.318538</f>
+      <c r="K10" s="7" t="n">
+        <f aca="false">J10*100/1.318538</f>
         <v>-19.5767585007031</v>
       </c>
     </row>
@@ -677,18 +711,21 @@
       <c r="F11" s="8" t="n">
         <v>-1.121774</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>12</v>
+      <c r="G11" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="8" t="n">
+      <c r="I11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="8" t="n">
         <f aca="false">B11-F11</f>
         <v>0.0103740000000001</v>
       </c>
-      <c r="J11" s="10" t="n">
-        <f aca="false">I11*100/1.318538</f>
+      <c r="K11" s="10" t="n">
+        <f aca="false">J11*100/1.318538</f>
         <v>0.786780509928429</v>
       </c>
     </row>
@@ -711,18 +748,21 @@
       <c r="F12" s="8" t="n">
         <v>-1.006976</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>12</v>
+      <c r="G12" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="8" t="n">
+      <c r="I12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="8" t="n">
         <f aca="false">B12-F12</f>
         <v>-0.0167539999999999</v>
       </c>
-      <c r="J12" s="10" t="n">
-        <f aca="false">I12*100/1.318538</f>
+      <c r="K12" s="10" t="n">
+        <f aca="false">J12*100/1.318538</f>
         <v>-1.27064976511863</v>
       </c>
     </row>
@@ -745,18 +785,21 @@
       <c r="F13" s="8" t="n">
         <v>-0.974515</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>12</v>
+      <c r="G13" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="8" t="n">
+      <c r="I13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="8" t="n">
         <f aca="false">B13-F13</f>
         <v>0.013725</v>
       </c>
-      <c r="J13" s="10" t="n">
-        <f aca="false">I13*100/1.318538</f>
+      <c r="K13" s="10" t="n">
+        <f aca="false">J13*100/1.318538</f>
         <v>1.04092563126736</v>
       </c>
     </row>
@@ -779,18 +822,21 @@
       <c r="F14" s="8" t="n">
         <v>-0.847607</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>12</v>
+      <c r="G14" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="8" t="n">
+      <c r="I14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="8" t="n">
         <f aca="false">B14-F14</f>
         <v>-0.049033</v>
       </c>
-      <c r="J14" s="10" t="n">
-        <f aca="false">I14*100/1.318538</f>
+      <c r="K14" s="10" t="n">
+        <f aca="false">J14*100/1.318538</f>
         <v>-3.71873999839216</v>
       </c>
     </row>
@@ -813,18 +859,21 @@
       <c r="F15" s="8" t="n">
         <v>-0.816774</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>12</v>
+      <c r="G15" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="8" t="n">
+      <c r="I15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="8" t="n">
         <f aca="false">B15-F15</f>
         <v>-0.00809599999999999</v>
       </c>
-      <c r="J15" s="10" t="n">
-        <f aca="false">I15*100/1.318538</f>
+      <c r="K15" s="10" t="n">
+        <f aca="false">J15*100/1.318538</f>
         <v>-0.614013399689656</v>
       </c>
     </row>
@@ -847,18 +896,21 @@
       <c r="F16" s="8" t="n">
         <v>-0.748681</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>12</v>
+      <c r="G16" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="8" t="n">
+      <c r="I16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="8" t="n">
         <f aca="false">B16-F16</f>
         <v>0.015891</v>
       </c>
-      <c r="J16" s="10" t="n">
-        <f aca="false">I16*100/1.318538</f>
+      <c r="K16" s="10" t="n">
+        <f aca="false">J16*100/1.318538</f>
         <v>1.20519848498868</v>
       </c>
     </row>
@@ -881,18 +933,21 @@
       <c r="F17" s="8" t="n">
         <v>-0.713119</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>12</v>
+      <c r="G17" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="8" t="n">
+      <c r="I17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="8" t="n">
         <f aca="false">B17-F17</f>
         <v>-0.0584210000000001</v>
       </c>
-      <c r="J17" s="10" t="n">
-        <f aca="false">I17*100/1.318538</f>
+      <c r="K17" s="10" t="n">
+        <f aca="false">J17*100/1.318538</f>
         <v>-4.43074071433664</v>
       </c>
     </row>
@@ -915,18 +970,21 @@
       <c r="F18" s="8" t="n">
         <v>-0.674879</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>12</v>
+      <c r="G18" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="8" t="n">
+      <c r="I18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="8" t="n">
         <f aca="false">B18-F18</f>
         <v>-0.0488909999999999</v>
       </c>
-      <c r="J18" s="10" t="n">
-        <f aca="false">I18*100/1.318538</f>
+      <c r="K18" s="10" t="n">
+        <f aca="false">J18*100/1.318538</f>
         <v>-3.70797049459325</v>
       </c>
     </row>
@@ -949,18 +1007,21 @@
       <c r="F19" s="8" t="n">
         <v>-0.658624</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>12</v>
+      <c r="G19" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="8" t="n">
+      <c r="I19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="8" t="n">
         <f aca="false">B19-F19</f>
         <v>-0.0485059999999999</v>
       </c>
-      <c r="J19" s="10" t="n">
-        <f aca="false">I19*100/1.318538</f>
+      <c r="K19" s="10" t="n">
+        <f aca="false">J19*100/1.318538</f>
         <v>-3.67877148781453</v>
       </c>
     </row>
@@ -983,18 +1044,21 @@
       <c r="F20" s="5" t="n">
         <v>-0.551624</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>10</v>
+      <c r="G20" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="5" t="n">
+      <c r="I20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="5" t="n">
         <f aca="false">B20-F20</f>
         <v>-0.137066</v>
       </c>
-      <c r="J20" s="7" t="n">
-        <f aca="false">I20*100/1.318538</f>
+      <c r="K20" s="7" t="n">
+        <f aca="false">J20*100/1.318538</f>
         <v>-10.3953014626806</v>
       </c>
     </row>
@@ -1017,18 +1081,21 @@
       <c r="F21" s="8" t="n">
         <v>-0.619345</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>12</v>
+      <c r="G21" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="8" t="n">
+      <c r="I21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="8" t="n">
         <f aca="false">B21-F21</f>
         <v>-0.0302450000000001</v>
       </c>
-      <c r="J21" s="10" t="n">
-        <f aca="false">I21*100/1.318538</f>
+      <c r="K21" s="10" t="n">
+        <f aca="false">J21*100/1.318538</f>
         <v>-2.29382846759063</v>
       </c>
     </row>
@@ -1051,18 +1118,21 @@
       <c r="F22" s="8" t="n">
         <v>-0.602197</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>12</v>
+      <c r="G22" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="8" t="n">
+      <c r="I22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="8" t="n">
         <f aca="false">B22-F22</f>
         <v>-0.032873</v>
       </c>
-      <c r="J22" s="10" t="n">
-        <f aca="false">I22*100/1.318538</f>
+      <c r="K22" s="10" t="n">
+        <f aca="false">J22*100/1.318538</f>
         <v>-2.4931401294464</v>
       </c>
     </row>
@@ -1085,18 +1155,21 @@
       <c r="F23" s="5" t="n">
         <v>-0.461595</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>10</v>
+      <c r="G23" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I23" s="5" t="n">
+      <c r="I23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="5" t="n">
         <f aca="false">B23-F23</f>
         <v>-0.168295</v>
       </c>
-      <c r="J23" s="7" t="n">
-        <f aca="false">I23*100/1.318538</f>
+      <c r="K23" s="7" t="n">
+        <f aca="false">J23*100/1.318538</f>
         <v>-12.7637580411031</v>
       </c>
     </row>
@@ -1119,18 +1192,21 @@
       <c r="F24" s="5" t="n">
         <v>-0.461584</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>10</v>
+      <c r="G24" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="5" t="n">
+      <c r="I24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="5" t="n">
         <f aca="false">B24-F24</f>
         <v>-0.099186</v>
       </c>
-      <c r="J24" s="7" t="n">
-        <f aca="false">I24*100/1.318538</f>
+      <c r="K24" s="7" t="n">
+        <f aca="false">J24*100/1.318538</f>
         <v>-7.52242256195878</v>
       </c>
     </row>
@@ -1153,18 +1229,21 @@
       <c r="F25" s="5" t="n">
         <v>-0.425409</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>10</v>
+      <c r="G25" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="I25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="5" t="n">
         <f aca="false">B25-F25</f>
         <v>-0.148711</v>
       </c>
-      <c r="J25" s="7" t="n">
-        <f aca="false">I25*100/1.318538</f>
+      <c r="K25" s="7" t="n">
+        <f aca="false">J25*100/1.318538</f>
         <v>-11.2784766157669</v>
       </c>
     </row>
@@ -1187,18 +1266,21 @@
       <c r="F26" s="8" t="n">
         <v>-0.589515</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>12</v>
+      <c r="G26" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="8" t="n">
+      <c r="I26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="8" t="n">
         <f aca="false">B26-F26</f>
         <v>0.039305</v>
       </c>
-      <c r="J26" s="10" t="n">
-        <f aca="false">I26*100/1.318538</f>
+      <c r="K26" s="10" t="n">
+        <f aca="false">J26*100/1.318538</f>
         <v>2.98095314659115</v>
       </c>
     </row>
@@ -1221,18 +1303,21 @@
       <c r="F27" s="8" t="n">
         <v>-0.488601</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>12</v>
+      <c r="G27" s="8" t="n">
+        <v>2</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="8" t="n">
+      <c r="I27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="8" t="n">
         <f aca="false">B27-F27</f>
         <v>0.0302309999999999</v>
       </c>
-      <c r="J27" s="10" t="n">
-        <f aca="false">I27*100/1.318538</f>
+      <c r="K27" s="10" t="n">
+        <f aca="false">J27*100/1.318538</f>
         <v>2.29276668552593</v>
       </c>
     </row>
@@ -1255,17 +1340,20 @@
       <c r="F28" s="8" t="n">
         <v>-0.486108</v>
       </c>
-      <c r="G28" s="9" t="s">
-        <v>12</v>
+      <c r="G28" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I28" s="8" t="n">
+      <c r="I28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="8" t="n">
         <f aca="false">B28-F28</f>
         <v>0.016858</v>
       </c>
-      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="n">
@@ -1286,17 +1374,20 @@
       <c r="F29" s="8" t="n">
         <v>-0.349774</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>12</v>
+      <c r="G29" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="8" t="n">
+      <c r="I29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="8" t="n">
         <f aca="false">B29-F29</f>
         <v>0.053834</v>
       </c>
-      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
@@ -1317,17 +1408,20 @@
       <c r="F30" s="5" t="n">
         <v>-0.022965</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>10</v>
+      <c r="G30" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="5" t="n">
+      <c r="I30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="5" t="n">
         <f aca="false">B30-F30</f>
         <v>-0.258365</v>
       </c>
-      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="n">
@@ -1348,17 +1442,20 @@
       <c r="F31" s="8" t="n">
         <v>-0.243236</v>
       </c>
-      <c r="G31" s="9" t="s">
-        <v>12</v>
+      <c r="G31" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="8" t="n">
         <f aca="false">B31-F31</f>
         <v>0.040686</v>
       </c>
-      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
@@ -1379,17 +1476,20 @@
       <c r="F32" s="5" t="n">
         <v>-0.022962</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>10</v>
+      <c r="G32" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I32" s="5" t="n">
+      <c r="I32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="5" t="n">
         <f aca="false">B32-F32</f>
         <v>-0.152828</v>
       </c>
-      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="n">
@@ -1410,17 +1510,20 @@
       <c r="F33" s="8" t="n">
         <v>-0.218151</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>12</v>
+      <c r="G33" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="8" t="n">
+      <c r="I33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="8" t="n">
         <f aca="false">B33-F33</f>
         <v>0.118621</v>
       </c>
-      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="n">
@@ -1441,17 +1544,20 @@
       <c r="F34" s="8" t="n">
         <v>-0.089588</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>12</v>
+      <c r="G34" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="8" t="n">
+      <c r="I34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="8" t="n">
         <f aca="false">B34-F34</f>
         <v>0.056998</v>
       </c>
-      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="n">
@@ -1472,17 +1578,20 @@
       <c r="F35" s="8" t="n">
         <v>-0.073242</v>
       </c>
-      <c r="G35" s="9" t="s">
-        <v>12</v>
+      <c r="G35" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I35" s="8" t="n">
+      <c r="I35" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="8" t="n">
         <f aca="false">B35-F35</f>
         <v>0.047252</v>
       </c>
-      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="n">
@@ -1503,17 +1612,20 @@
       <c r="F36" s="8" t="n">
         <v>-0.054358</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>12</v>
+      <c r="G36" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="8" t="n">
+      <c r="I36" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="8" t="n">
         <f aca="false">B36-F36</f>
         <v>0.048628</v>
       </c>
-      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="n">
@@ -1534,17 +1646,20 @@
       <c r="F37" s="8" t="n">
         <v>-0.034471</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>12</v>
+      <c r="G37" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="8" t="n">
+      <c r="I37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="8" t="n">
         <f aca="false">B37-F37</f>
         <v>0.052781</v>
       </c>
-      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="n">
@@ -1565,17 +1680,20 @@
       <c r="F38" s="8" t="n">
         <v>-0.012115</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>12</v>
+      <c r="G38" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="8" t="n">
         <f aca="false">B38-F38</f>
         <v>-0.028615</v>
       </c>
-      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="n">
@@ -1596,17 +1714,20 @@
       <c r="F39" s="8" t="n">
         <v>-0.006079</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>12</v>
+      <c r="G39" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="8" t="n">
+      <c r="I39" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="8" t="n">
         <f aca="false">B39-F39</f>
         <v>0.024969</v>
       </c>
-      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="n">
@@ -1627,17 +1748,20 @@
       <c r="F40" s="8" t="n">
         <v>0.04884</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>12</v>
+      <c r="G40" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="8" t="n">
+      <c r="I40" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="8" t="n">
         <f aca="false">B40-F40</f>
         <v>0.01875</v>
       </c>
-      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="n">
@@ -1658,17 +1782,20 @@
       <c r="F41" s="8" t="n">
         <v>0.052907</v>
       </c>
-      <c r="G41" s="9" t="s">
-        <v>12</v>
+      <c r="G41" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="8" t="n">
+      <c r="I41" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="8" t="n">
         <f aca="false">B41-F41</f>
         <v>0.052643</v>
       </c>
-      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="n">
@@ -1689,21 +1816,24 @@
       <c r="F42" s="8" t="n">
         <v>0.105619</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>12</v>
+      <c r="G42" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I42" s="8" t="n">
+      <c r="I42" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="8" t="n">
         <f aca="false">B42-F42</f>
         <v>0.018651</v>
       </c>
-      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B44" s="12" t="n">
         <f aca="false">SUM(B1:B27)</f>
@@ -1717,13 +1847,14 @@
         <f aca="false">SUM(F1:F27)</f>
         <v>-104.458172</v>
       </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="12" t="n">
-        <f aca="false">SUM(I1:I27)</f>
+      <c r="G44" s="12"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="12" t="n">
+        <f aca="false">SUM(J1:J27)</f>
         <v>-1.318538</v>
       </c>
-      <c r="J44" s="13" t="n">
-        <f aca="false">SUM(J1:J27)</f>
+      <c r="K44" s="13" t="n">
+        <f aca="false">SUM(K1:K27)</f>
         <v>-100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make diagram for 4-MeOPhN2+
</commit_message>
<xml_diff>
--- a/bin/Ph-N2+-MTMO-transform.xlsx
+++ b/bin/Ph-N2+-MTMO-transform.xlsx
@@ -304,21 +304,21 @@
   </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:I"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="38.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="1" width="38.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>

</xml_diff>